<commit_message>
false recognition error fix, dfa transition table typo fix
</commit_message>
<xml_diff>
--- a/DFA_Transition_Table.xlsx
+++ b/DFA_Transition_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\중앙대학교\3학년 1학기\컴파일러\과제\compiler-lexical-analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75613B2-8075-4724-AC3B-6F44E80A5705}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AFD0F0-1F35-4D2A-AC87-FAAB8781A689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6586DD6C-782B-4D00-89E9-AB0FE2F93306}"/>
   </bookViews>
@@ -1430,8 +1430,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6A950B-FFA9-47F3-97C4-65B7CB8C91CD}">
   <dimension ref="C4:CI89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX51" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BS71" sqref="BS71"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="BB52" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="BM76" sqref="BM76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -9851,10 +9854,10 @@
         <v>166</v>
       </c>
       <c r="AG42" s="1" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="AH42" s="1" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="AI42" s="1" t="s">
         <v>166</v>

</xml_diff>